<commit_message>
.ods support: Assume UTC for naive dates as we do for xlsx
</commit_message>
<xml_diff>
--- a/flattentool/tests/fixtures/xlsx/types.xlsx
+++ b/flattentool/tests/fixtures/xlsx/types.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">colInt</t>
   </si>
@@ -30,21 +30,24 @@
   <si>
     <t xml:space="preserve">colDate</t>
   </si>
+  <si>
+    <t xml:space="preserve">colDateTime</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY\ HH:MM"/>
   </numFmts>
-  <fonts count="4">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+  <fonts count="16">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -61,16 +64,135 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -78,8 +200,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -103,8 +240,59 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -113,16 +301,128 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{2540C00B-3C0A-44DC-82CB-60D22D5A0619}">
+  <header guid="{2540C00B-3C0A-44DC-82CB-60D22D5A0619}" dateTime="2020-02-07T16:56:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="4" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rrc rId="1" ua="false" sId="1" eol="0" ref="E:E" action="deleteCol">
+    <rfmt sheetId="1" sqref="E:E"/>
+  </rrc>
+  <rrc rId="2" ua="false" sId="1" eol="0" ref="E:E" action="deleteCol">
+    <rfmt sheetId="1" sqref="E:E"/>
+  </rrc>
+  <rrc rId="3" ua="false" sId="1" eol="0" ref="E:E" action="deleteCol">
+    <rfmt sheetId="1" sqref="E:E"/>
+  </rrc>
+  <rrc rId="4" ua="false" sId="1" eol="0" ref="E:E" action="deleteCol">
+    <rfmt sheetId="1" sqref="E:E"/>
+  </rrc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -131,15 +431,17 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C2"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -152,6 +454,9 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -162,6 +467,9 @@
       </c>
       <c r="C2" s="1" t="n">
         <v>43895</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>43868.6951388889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ODSReader: Parse numbers correctly from .ods files
https://github.com/OpenDataServices/flatten-tool/issues/343
</commit_message>
<xml_diff>
--- a/flattentool/tests/fixtures/xlsx/types.xlsx
+++ b/flattentool/tests/fixtures/xlsx/types.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">colInt</t>
   </si>
   <si>
     <t xml:space="preserve">colFloat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colFloatComma</t>
   </si>
   <si>
     <t xml:space="preserve">colDate</t>
@@ -38,10 +41,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY\ HH:MM"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,###.00"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="168" formatCode="DD/MM/YY\ HH:MM"/>
+    <numFmt numFmtId="169" formatCode="HH:MM:SS"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -292,7 +298,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -302,6 +308,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,54 +412,24 @@
 </styleSheet>
 </file>
 
-<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{2540C00B-3C0A-44DC-82CB-60D22D5A0619}">
-  <header guid="{2540C00B-3C0A-44DC-82CB-60D22D5A0619}" dateTime="2020-02-07T16:56:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="4" maxSheetId="2">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-</headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rrc rId="1" ua="false" sId="1" eol="0" ref="E:E" action="deleteCol">
-    <rfmt sheetId="1" sqref="E:E"/>
-  </rrc>
-  <rrc rId="2" ua="false" sId="1" eol="0" ref="E:E" action="deleteCol">
-    <rfmt sheetId="1" sqref="E:E"/>
-  </rrc>
-  <rrc rId="3" ua="false" sId="1" eol="0" ref="E:E" action="deleteCol">
-    <rfmt sheetId="1" sqref="E:E"/>
-  </rrc>
-  <rrc rId="4" ua="false" sId="1" eol="0" ref="E:E" action="deleteCol">
-    <rfmt sheetId="1" sqref="E:E"/>
-  </rrc>
-</revisions>
-</file>
-
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -457,20 +445,28 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="B2" s="1" t="n">
+        <v>1000.2</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1000.2</v>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>43895</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="E2" s="4" t="n">
         <v>43868.6951388889</v>
       </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>